<commit_message>
Fix saving schedules and reports
</commit_message>
<xml_diff>
--- a/timetables/plan_1.xlsx
+++ b/timetables/plan_1.xlsx
@@ -584,7 +584,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Podstawy programowania (CWL)</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -675,7 +675,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Podstawy programowania (CWL)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">

</xml_diff>